<commit_message>
New Data is added
</commit_message>
<xml_diff>
--- a/src/main/java/com/ep/test/data/TestData.xlsx
+++ b/src/main/java/com/ep/test/data/TestData.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="4140"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="4140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="StudentForm" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:L12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Login</t>
   </si>
@@ -32,13 +32,118 @@
   </si>
   <si>
     <t>mani6747@gmail.com</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua </t>
+  </si>
+  <si>
+    <t>Middlename</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Studentid</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Emailaddress</t>
+  </si>
+  <si>
+    <t>Parentemployer</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Relationtochild</t>
+  </si>
+  <si>
+    <t>Pickuppersonname</t>
+  </si>
+  <si>
+    <t>PickuppersonTelephone</t>
+  </si>
+  <si>
+    <t>Jhon</t>
+  </si>
+  <si>
+    <t>979-87-8787</t>
+  </si>
+  <si>
+    <t>K4</t>
+  </si>
+  <si>
+    <t>3217 Versante Drive</t>
+  </si>
+  <si>
+    <t>965-679-8989</t>
+  </si>
+  <si>
+    <t>966-659-7666</t>
+  </si>
+  <si>
+    <t>IT Industry</t>
+  </si>
+  <si>
+    <t>Daren</t>
+  </si>
+  <si>
+    <t>Uncel</t>
+  </si>
+  <si>
+    <t>Josep</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Manikanta</t>
+  </si>
+  <si>
+    <t>StudentForm</t>
+  </si>
+  <si>
+    <t>ParentorGuardian</t>
+  </si>
+  <si>
+    <t>SignatureLegalParentorGuardian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +157,19 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,12 +196,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -381,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,13 +561,239 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>912</v>
+      </c>
+      <c r="H4" s="4">
+        <v>38880</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4">
+        <v>38119</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
New data for signup is added
</commit_message>
<xml_diff>
--- a/src/main/java/com/ep/test/data/TestData.xlsx
+++ b/src/main/java/com/ep/test/data/TestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="4140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="5040"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="StudentForm" sheetId="2" r:id="rId2"/>
+    <sheet name="Signup" sheetId="3" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId2"/>
+    <sheet name="StudentForm" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="S1:AA12"/>
+  <oleSize ref="A1:M15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>Login</t>
   </si>
@@ -162,7 +163,37 @@
     <t>Mayank</t>
   </si>
   <si>
-    <t>ebiztesting8@gmail.com</t>
+    <t>Signup</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Mason</t>
+  </si>
+  <si>
+    <t>williams</t>
+  </si>
+  <si>
+    <t>6136 Walraven Cir</t>
+  </si>
+  <si>
+    <t>jamesrobert441@gmail.com</t>
+  </si>
+  <si>
+    <t>Memphis</t>
   </si>
 </sst>
 </file>
@@ -172,7 +203,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,21 +237,55 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -231,7 +296,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -244,6 +309,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -539,10 +608,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4">
+        <v>123456</v>
+      </c>
+      <c r="H4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4">
+        <v>38119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>123456</v>
@@ -598,12 +782,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="E8:F8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
New Test data is added
</commit_message>
<xml_diff>
--- a/src/main/java/com/ep/test/data/TestData.xlsx
+++ b/src/main/java/com/ep/test/data/TestData.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="5040"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="5040" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="3" r:id="rId1"/>
     <sheet name="Login" sheetId="1" r:id="rId2"/>
     <sheet name="StudentForm" sheetId="2" r:id="rId3"/>
+    <sheet name="Contactus" sheetId="4" r:id="rId4"/>
+    <sheet name="ChangePassword" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:M15"/>
+  <oleSize ref="A1:L15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>Login</t>
   </si>
@@ -194,6 +196,48 @@
   </si>
   <si>
     <t>Memphis</t>
+  </si>
+  <si>
+    <t>Contactus</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>mailid</t>
+  </si>
+  <si>
+    <t>Ph</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Thota</t>
+  </si>
+  <si>
+    <t>eBiz Solutions</t>
+  </si>
+  <si>
+    <t>This sample checking for contact us</t>
+  </si>
+  <si>
+    <t>ChangePassword</t>
+  </si>
+  <si>
+    <t>CurrentPassword</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>mani123</t>
   </si>
 </sst>
 </file>
@@ -610,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -726,7 +770,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1065,4 +1109,180 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4">
+        <v>38119</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4">
+        <v>1234567</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New Testdata is added
</commit_message>
<xml_diff>
--- a/src/main/java/com/ep/test/data/TestData.xlsx
+++ b/src/main/java/com/ep/test/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="5040" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15135" windowHeight="5040"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="3" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="ChangePassword" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L15"/>
+  <oleSize ref="A1:J15"/>
 </workbook>
 </file>
 
@@ -654,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -830,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -1232,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New Code is added to generate excel reports
</commit_message>
<xml_diff>
--- a/src/main/java/com/ep/test/data/TestData.xlsx
+++ b/src/main/java/com/ep/test/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15435" windowHeight="5040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15240" windowHeight="4410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="149">
   <si>
     <t>Login</t>
   </si>
@@ -471,10 +471,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +528,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -571,14 +580,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -612,8 +622,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -910,7 +930,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,17 +1055,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1055,44 +1075,48 @@
       <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="30" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13">
-        <v>123456</v>
-      </c>
+      <c r="C4" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Need to enter URL in this file
Change-Id: I371ab0932bc7830565862ca86f9c45b8188fdffe
Signed-off-by: rajasekhar.alm@gmail.com
</commit_message>
<xml_diff>
--- a/src/main/java/com/ep/test/data/TestData.xlsx
+++ b/src/main/java/com/ep/test/data/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BE14793A-F5C9-42DC-8630-7D3F1F278D0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15420" windowHeight="2280" tabRatio="377" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="2880" tabRatio="377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="3" r:id="rId1"/>
@@ -13,7 +14,8 @@
     <sheet name="Contactus" sheetId="4" r:id="rId4"/>
     <sheet name="ChangePassword" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M7"/>
 </workbook>
 </file>
 
@@ -488,12 +490,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,6 +671,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -715,7 +725,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,9 +757,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -781,6 +809,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -956,14 +1002,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -977,7 +1023,7 @@
     <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="21">
         <v>0</v>
       </c>
@@ -1006,7 +1052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -1019,7 +1065,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1048,7 +1094,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1084,21 +1130,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1109,14 +1155,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="24"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -1127,7 +1173,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1138,12 +1184,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1151,14 +1197,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:PD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+    <sheetView topLeftCell="BC1" workbookViewId="0">
       <selection activeCell="BK11" sqref="BK11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1219,7 +1265,7 @@
     <col min="64" max="420" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:420">
+    <row r="1" spans="1:420" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1410,7 +1456,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:420" s="11" customFormat="1">
+    <row r="2" spans="1:420" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
@@ -1775,7 +1821,7 @@
       <c r="PC2" s="32"/>
       <c r="PD2" s="32"/>
     </row>
-    <row r="3" spans="1:420" s="11" customFormat="1">
+    <row r="3" spans="1:420" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -2323,7 +2369,7 @@
       <c r="PC3" s="32"/>
       <c r="PD3" s="32"/>
     </row>
-    <row r="4" spans="1:420" s="11" customFormat="1" ht="15.75">
+    <row r="4" spans="1:420" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
@@ -2871,26 +2917,26 @@
       <c r="PC4" s="32"/>
       <c r="PD4" s="32"/>
     </row>
-    <row r="5" spans="1:420" ht="15.75">
+    <row r="5" spans="1:420" ht="15.75" x14ac:dyDescent="0.25">
       <c r="BB5" s="4"/>
     </row>
-    <row r="10" spans="1:420" ht="15.75">
+    <row r="10" spans="1:420" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F10" s="26"/>
     </row>
-    <row r="11" spans="1:420" ht="15.75">
+    <row r="11" spans="1:420" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:420" ht="15.75">
+    <row r="12" spans="1:420" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D12" s="26"/>
     </row>
-    <row r="17" spans="6:6" ht="15.75">
+    <row r="17" spans="6:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F17" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2" display="http://nameberry.com/babyname/William"/>
-    <hyperlink ref="U4" r:id="rId3"/>
+    <hyperlink ref="N4" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" display="http://nameberry.com/babyname/William" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="U4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2898,14 +2944,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -2916,7 +2962,7 @@
     <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2942,7 +2988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
@@ -2954,7 +3000,7 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -2980,7 +3026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>36</v>
       </c>
@@ -3008,7 +3054,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3016,14 +3062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -3031,7 +3077,7 @@
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3042,14 +3088,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -3060,7 +3106,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>39</v>
       </c>

</xml_diff>